<commit_message>
Updated CHE model - 2025-08-08 12:16
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F8A62F-FC9B-421F-8066-57F5375D2A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{857A1E1F-C170-415C-A87C-8291CFB3E802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Veda" sheetId="1" r:id="rId1"/>
-    <sheet name="historical_data_long" sheetId="3" r:id="rId2"/>
+    <sheet name="grids_capacity" sheetId="4" r:id="rId1"/>
+    <sheet name="Veda" sheetId="1" r:id="rId2"/>
+    <sheet name="historical_data_long" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="288">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -327,6 +328,639 @@
   </si>
   <si>
     <t>UC_RHSRT~2050</t>
+  </si>
+  <si>
+    <t>pasti</t>
+  </si>
+  <si>
+    <t>g_CH1-220-CH2-220</t>
+  </si>
+  <si>
+    <t>g_CH11-220-w147557680-220</t>
+  </si>
+  <si>
+    <t>g_CH12-220-w207993342-220</t>
+  </si>
+  <si>
+    <t>g_CH12-380-w207993342-380</t>
+  </si>
+  <si>
+    <t>g_CH13-220-CH12-220</t>
+  </si>
+  <si>
+    <t>g_CH13-220-w52738225-220</t>
+  </si>
+  <si>
+    <t>g_CH14-220-w212722603-220</t>
+  </si>
+  <si>
+    <t>g_CH14-220-w402053379-220</t>
+  </si>
+  <si>
+    <t>g_CH14-380-w50319857-380</t>
+  </si>
+  <si>
+    <t>g_CH15-220-w159527493-220</t>
+  </si>
+  <si>
+    <t>g_CH15-220-w97941869-220</t>
+  </si>
+  <si>
+    <t>g_CH17-380-w71500123-380</t>
+  </si>
+  <si>
+    <t>g_CH18-380-CH16-380</t>
+  </si>
+  <si>
+    <t>g_CH19-220-CH14-220</t>
+  </si>
+  <si>
+    <t>g_CH19-220-CH20-220</t>
+  </si>
+  <si>
+    <t>g_CH2-220-w50319857-220</t>
+  </si>
+  <si>
+    <t>g_CH20-220-CH19-220</t>
+  </si>
+  <si>
+    <t>g_CH21-220-w36348118-220</t>
+  </si>
+  <si>
+    <t>g_CH22-380-CH29-380</t>
+  </si>
+  <si>
+    <t>g_CH23-220-CH24-220</t>
+  </si>
+  <si>
+    <t>g_CH24-220-CH26-220</t>
+  </si>
+  <si>
+    <t>g_CH25-220-w240959264-220</t>
+  </si>
+  <si>
+    <t>g_CH26-220-CH28-220</t>
+  </si>
+  <si>
+    <t>g_CH27-220-CH25-220</t>
+  </si>
+  <si>
+    <t>g_CH27-220-w1086214433-220</t>
+  </si>
+  <si>
+    <t>g_CH28-220-w431234146-220</t>
+  </si>
+  <si>
+    <t>g_CH3-220-w281809991-220</t>
+  </si>
+  <si>
+    <t>g_CH30-380-CH33-380</t>
+  </si>
+  <si>
+    <t>g_CH30-380-w208780268-380</t>
+  </si>
+  <si>
+    <t>g_CH31-220-w132373704-220</t>
+  </si>
+  <si>
+    <t>g_CH32-220-w281803398-220</t>
+  </si>
+  <si>
+    <t>g_CH33-380-CH37-380</t>
+  </si>
+  <si>
+    <t>g_CH34-220-CH35-220</t>
+  </si>
+  <si>
+    <t>g_CH36-220-CH27-220</t>
+  </si>
+  <si>
+    <t>g_CH36-220-CH39-220</t>
+  </si>
+  <si>
+    <t>g_CH37-380-w207991759-380</t>
+  </si>
+  <si>
+    <t>g_CH38-220-CH39-220</t>
+  </si>
+  <si>
+    <t>g_CH38-220-w1092884227-220</t>
+  </si>
+  <si>
+    <t>g_CH39-220-CH36-220</t>
+  </si>
+  <si>
+    <t>g_CH4-220-CH9-220</t>
+  </si>
+  <si>
+    <t>g_CH4-220-w92873516-220</t>
+  </si>
+  <si>
+    <t>g_CH40-220-CH35-220</t>
+  </si>
+  <si>
+    <t>g_CH41-380-w207993342-380</t>
+  </si>
+  <si>
+    <t>g_CH41-380-w281804158-380</t>
+  </si>
+  <si>
+    <t>g_CH42-220-w969811258-220</t>
+  </si>
+  <si>
+    <t>g_CH43-220-CH44-220</t>
+  </si>
+  <si>
+    <t>g_CH43-220-w402055336-220</t>
+  </si>
+  <si>
+    <t>g_CH44-220-w234983117-220</t>
+  </si>
+  <si>
+    <t>g_CH45-220-CH29-220</t>
+  </si>
+  <si>
+    <t>g_CH46-220-CH47-220</t>
+  </si>
+  <si>
+    <t>g_CH47-220-w212722603-220</t>
+  </si>
+  <si>
+    <t>g_CH49-225-CH48-225</t>
+  </si>
+  <si>
+    <t>g_CH5-220-w89977424-220</t>
+  </si>
+  <si>
+    <t>g_CH50-220-w281804158-220</t>
+  </si>
+  <si>
+    <t>g_CH53-225-CH49-225</t>
+  </si>
+  <si>
+    <t>g_CH53-225-w55698557-225</t>
+  </si>
+  <si>
+    <t>g_CH56-220-CH58-220</t>
+  </si>
+  <si>
+    <t>g_CH56-220-w281815404-220</t>
+  </si>
+  <si>
+    <t>g_CH59-220-w281800404-220</t>
+  </si>
+  <si>
+    <t>g_CH6-220-CH3-220</t>
+  </si>
+  <si>
+    <t>g_CH60-225-CH53-225</t>
+  </si>
+  <si>
+    <t>g_CH7-220-w89405664-220</t>
+  </si>
+  <si>
+    <t>g_CH9-220-w455120191-220</t>
+  </si>
+  <si>
+    <t>g_r5378910-220-w1105061707-220</t>
+  </si>
+  <si>
+    <t>g_r7933294-380-CH30-380</t>
+  </si>
+  <si>
+    <t>g_r9310861-220-w11282314-220</t>
+  </si>
+  <si>
+    <t>g_w100662075-220-w210568055-220</t>
+  </si>
+  <si>
+    <t>g_w108257952-220-w33271433-220</t>
+  </si>
+  <si>
+    <t>g_w108257952-220-w35002638-220</t>
+  </si>
+  <si>
+    <t>g_w109037817-220-CH2-220</t>
+  </si>
+  <si>
+    <t>g_w109037817-380-w397960460-380</t>
+  </si>
+  <si>
+    <t>g_w1105061707-220-CH14-220</t>
+  </si>
+  <si>
+    <t>g_w1105061707-220-w402053379-220</t>
+  </si>
+  <si>
+    <t>g_w1105061707-220-w402055336-220</t>
+  </si>
+  <si>
+    <t>g_w111162936-220-CH31-220</t>
+  </si>
+  <si>
+    <t>g_w111162936-220-w55698557-220</t>
+  </si>
+  <si>
+    <t>g_w111162936-380-w936521586-380</t>
+  </si>
+  <si>
+    <t>g_w11282314-220-CH12-220</t>
+  </si>
+  <si>
+    <t>g_w11282314-220-CH6-220</t>
+  </si>
+  <si>
+    <t>g_w1208713169-220-w207993342-220</t>
+  </si>
+  <si>
+    <t>g_w1208713169-220-w212498548-220</t>
+  </si>
+  <si>
+    <t>g_w122720993-220-w1105061707-220</t>
+  </si>
+  <si>
+    <t>g_w127004407-380-CH14-380</t>
+  </si>
+  <si>
+    <t>g_w127004407-380-w1105061707-380</t>
+  </si>
+  <si>
+    <t>g_w127004407-380-w50319857-380</t>
+  </si>
+  <si>
+    <t>g_w1284913429-220-w165513396-220</t>
+  </si>
+  <si>
+    <t>g_w1327084723-220-CH42-220</t>
+  </si>
+  <si>
+    <t>g_w1327084723-220-w281800404-220</t>
+  </si>
+  <si>
+    <t>g_w140873735-220-CH23-220</t>
+  </si>
+  <si>
+    <t>g_w140873735-220-w130198336-220</t>
+  </si>
+  <si>
+    <t>g_w140873735-220-w35002638-220</t>
+  </si>
+  <si>
+    <t>g_w146225999-220-w35002638-220</t>
+  </si>
+  <si>
+    <t>g_w147557680-220-CH14-220</t>
+  </si>
+  <si>
+    <t>g_w147714395-220-CH3-220</t>
+  </si>
+  <si>
+    <t>g_w147714395-220-w22899676-220</t>
+  </si>
+  <si>
+    <t>g_w147714395-380-CH17-380</t>
+  </si>
+  <si>
+    <t>g_w147714395-380-w192677427-380</t>
+  </si>
+  <si>
+    <t>g_w148015471-220-r9310861-220</t>
+  </si>
+  <si>
+    <t>g_w148015471-220-w31308888-220</t>
+  </si>
+  <si>
+    <t>g_w159527493-220-w240959264-220</t>
+  </si>
+  <si>
+    <t>g_w161853746-220-r5378910-220</t>
+  </si>
+  <si>
+    <t>g_w161853746-220-w1105061707-220</t>
+  </si>
+  <si>
+    <t>g_w165254212-220-w147557680-220</t>
+  </si>
+  <si>
+    <t>g_w165513396-220-w33271433-220</t>
+  </si>
+  <si>
+    <t>g_w177392130-220-CH51-220</t>
+  </si>
+  <si>
+    <t>g_w177392130-220-CH52-220</t>
+  </si>
+  <si>
+    <t>g_w177392130-220-CH57-220</t>
+  </si>
+  <si>
+    <t>g_w177392130-400-CH51-400</t>
+  </si>
+  <si>
+    <t>g_w190819048-220-CH7-220</t>
+  </si>
+  <si>
+    <t>g_w190819048-220-w50319857-220</t>
+  </si>
+  <si>
+    <t>g_w192677427-220-CH13-220</t>
+  </si>
+  <si>
+    <t>g_w192677427-220-CH18-220</t>
+  </si>
+  <si>
+    <t>g_w192677427-220-w147714395-220</t>
+  </si>
+  <si>
+    <t>g_w192677427-220-w240575085-220</t>
+  </si>
+  <si>
+    <t>g_w192677427-380-CH16-380</t>
+  </si>
+  <si>
+    <t>g_w194258388-220-w122720993-220</t>
+  </si>
+  <si>
+    <t>g_w207993342-220-CH22-220</t>
+  </si>
+  <si>
+    <t>g_w208780268-380-w207993342-380</t>
+  </si>
+  <si>
+    <t>g_w209324991-220-w758315582-220</t>
+  </si>
+  <si>
+    <t>g_w210568055-220-w192677427-220</t>
+  </si>
+  <si>
+    <t>g_w210568055-220-w365556107-220</t>
+  </si>
+  <si>
+    <t>g_w210568055-380-CH16-380</t>
+  </si>
+  <si>
+    <t>g_w210568055-380-w71500123-380</t>
+  </si>
+  <si>
+    <t>g_w211907009-220-CH21-220</t>
+  </si>
+  <si>
+    <t>g_w211907009-220-w455120191-220</t>
+  </si>
+  <si>
+    <t>g_w212722603-220-w234983117-220</t>
+  </si>
+  <si>
+    <t>g_w212722603-220-w236819191-220</t>
+  </si>
+  <si>
+    <t>g_w212722603-380-w234983117-380</t>
+  </si>
+  <si>
+    <t>g_w22899676-220-CH3-220</t>
+  </si>
+  <si>
+    <t>g_w232662311-220-w111162936-220</t>
+  </si>
+  <si>
+    <t>g_w236819191-220-CH47-220</t>
+  </si>
+  <si>
+    <t>g_w236819191-220-w228003081-220</t>
+  </si>
+  <si>
+    <t>g_w238138373-380-w260211728-380</t>
+  </si>
+  <si>
+    <t>g_w239937062-220-CH52-220</t>
+  </si>
+  <si>
+    <t>g_w239937062-220-w132373704-220</t>
+  </si>
+  <si>
+    <t>g_w240575085-220-CH6-220</t>
+  </si>
+  <si>
+    <t>g_w240959264-220-CH20-220</t>
+  </si>
+  <si>
+    <t>g_w240959264-220-CH27-220</t>
+  </si>
+  <si>
+    <t>g_w240959264-220-w209324991-220</t>
+  </si>
+  <si>
+    <t>g_w242269161-220-CH14-220</t>
+  </si>
+  <si>
+    <t>g_w260211728-380-w936521586-380</t>
+  </si>
+  <si>
+    <t>g_w26166640-220-w758315582-220</t>
+  </si>
+  <si>
+    <t>g_w26843160-220-w92798668-220</t>
+  </si>
+  <si>
+    <t>g_w27107779-220-w147714395-220</t>
+  </si>
+  <si>
+    <t>g_w27435934-220-w109037817-220</t>
+  </si>
+  <si>
+    <t>g_w27435934-220-w30350721-220</t>
+  </si>
+  <si>
+    <t>g_w281799252-220-w52738225-220</t>
+  </si>
+  <si>
+    <t>g_w281800404-220-CH59-220</t>
+  </si>
+  <si>
+    <t>g_w281800404-220-w281815404-220</t>
+  </si>
+  <si>
+    <t>g_w281803398-220-CH50-220</t>
+  </si>
+  <si>
+    <t>g_w281809991-220-w26843160-220</t>
+  </si>
+  <si>
+    <t>g_w281815404-220-CH50-220</t>
+  </si>
+  <si>
+    <t>g_w281815404-220-CH58-220</t>
+  </si>
+  <si>
+    <t>g_w281815404-220-w35487135-220</t>
+  </si>
+  <si>
+    <t>g_w281822905-220-CH38-220</t>
+  </si>
+  <si>
+    <t>g_w281822905-220-CH42-220</t>
+  </si>
+  <si>
+    <t>g_w30350721-220-w356292116-220</t>
+  </si>
+  <si>
+    <t>g_w31308888-220-w89977424-220</t>
+  </si>
+  <si>
+    <t>g_w33271433-220-CH5-220</t>
+  </si>
+  <si>
+    <t>g_w35002638-220-CH15-220</t>
+  </si>
+  <si>
+    <t>g_w35002638-220-w140873735-220</t>
+  </si>
+  <si>
+    <t>g_w35002638-220-w242269161-220</t>
+  </si>
+  <si>
+    <t>g_w35002638-220-w281799252-220</t>
+  </si>
+  <si>
+    <t>g_w35002638-380-w52738225-380</t>
+  </si>
+  <si>
+    <t>g_w356292116-220-CH11-220</t>
+  </si>
+  <si>
+    <t>g_w356292116-220-w146225999-220</t>
+  </si>
+  <si>
+    <t>g_w356292116-220-w35002638-220</t>
+  </si>
+  <si>
+    <t>g_w356292116-220-w50319857-220</t>
+  </si>
+  <si>
+    <t>g_w356292116-380-w35002638-380</t>
+  </si>
+  <si>
+    <t>g_w356292116-380-w50319857-380</t>
+  </si>
+  <si>
+    <t>g_w35840165-380-w98648381-380</t>
+  </si>
+  <si>
+    <t>g_w364949845-220-w969819301-220</t>
+  </si>
+  <si>
+    <t>g_w364949845-380-CH34-380</t>
+  </si>
+  <si>
+    <t>g_w365556107-220-w71500123-220</t>
+  </si>
+  <si>
+    <t>g_w391577741-220-w391576135-220</t>
+  </si>
+  <si>
+    <t>g_w397960460-380-w50319857-380</t>
+  </si>
+  <si>
+    <t>g_w402053379-220-w190819048-220</t>
+  </si>
+  <si>
+    <t>g_w431234146-220-CH35-220</t>
+  </si>
+  <si>
+    <t>g_w431234146-220-w969811258-220</t>
+  </si>
+  <si>
+    <t>g_w44496892-220-CH31-220</t>
+  </si>
+  <si>
+    <t>g_w50319857-220-w98648381-220</t>
+  </si>
+  <si>
+    <t>g_w50319857-380-w35840165-380</t>
+  </si>
+  <si>
+    <t>g_w50319857-380-w98648381-380</t>
+  </si>
+  <si>
+    <t>g_w50561341-220-w147714395-220</t>
+  </si>
+  <si>
+    <t>g_w50561341-220-w87281514-220</t>
+  </si>
+  <si>
+    <t>g_w52738225-220-CH13-220</t>
+  </si>
+  <si>
+    <t>g_w52738225-380-CH12-380</t>
+  </si>
+  <si>
+    <t>g_w55695765-220-w111162936-220</t>
+  </si>
+  <si>
+    <t>g_w55698557-220-w194258388-220</t>
+  </si>
+  <si>
+    <t>g_w71500123-220-CH21-220</t>
+  </si>
+  <si>
+    <t>g_w71500123-380-w207993342-380</t>
+  </si>
+  <si>
+    <t>g_w758943072-220-w234983117-220</t>
+  </si>
+  <si>
+    <t>g_w802058337-220-w234983117-220</t>
+  </si>
+  <si>
+    <t>g_w802058337-220-w758943072-220</t>
+  </si>
+  <si>
+    <t>g_w802058337-225-CH60-225</t>
+  </si>
+  <si>
+    <t>g_w83861269-220-CH9-220</t>
+  </si>
+  <si>
+    <t>g_w89405664-220-w165513396-220</t>
+  </si>
+  <si>
+    <t>g_w89977424-220-CH5-220</t>
+  </si>
+  <si>
+    <t>g_w92798668-220-CH4-220</t>
+  </si>
+  <si>
+    <t>g_w92798668-220-w192677427-220</t>
+  </si>
+  <si>
+    <t>g_w92798668-220-w455120191-220</t>
+  </si>
+  <si>
+    <t>g_w936521586-380-w234983117-380</t>
+  </si>
+  <si>
+    <t>g_w969811258-380-w35002638-380</t>
+  </si>
+  <si>
+    <t>g_w969819301-220-CH46-220</t>
+  </si>
+  <si>
+    <t>g_w969819301-220-w391577741-220</t>
+  </si>
+  <si>
+    <t>g_w969819301-380-w364949845-380</t>
+  </si>
+  <si>
+    <t>g_w98648381-220-w165513396-220</t>
+  </si>
+  <si>
+    <t>g_w98648381-220-w27107779-220</t>
+  </si>
+  <si>
+    <t>g_w98648381-380-w147714395-380</t>
+  </si>
+  <si>
+    <t>g_w98648381-380-w165513396-380</t>
   </si>
 </sst>
 </file>
@@ -811,10 +1445,1720 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3922080-D7AB-4ED2-AEAD-43FE5570C1DF}">
+  <dimension ref="A1:B212"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="28.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1.4746679999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="11">
+        <v>1.4746679999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A51" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A52" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="13">
+        <v>1.0054560000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A55" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A56" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A57" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" s="11">
+        <v>1.005455</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A58" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="13">
+        <v>1.005455</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A59" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A61" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A62" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A63" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="11">
+        <v>1.005455</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A71" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A78" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A79" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B84" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B87" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B88" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B90" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B94" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B95" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B96" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A98" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B98" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A99" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A100" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B100" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A101" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B101" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A102" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A103" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A104" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B104" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A105" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B105" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A106" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B106" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A107" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B108" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B109" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B110" s="13">
+        <v>1.7874760000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A111" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B111" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A112" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B112" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B113" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B114" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B115" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B116" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B117" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B118" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B119" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A120" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B120" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B121" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A122" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B122" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A123" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B123" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A124" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B124" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A125" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B125" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A126" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B126" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A127" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B127" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A128" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B128" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A129" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B129" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A130" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B130" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A131" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B131" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A132" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B132" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A133" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B133" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A134" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B134" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B135" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B136" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B137" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B138" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A139" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B139" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A140" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B140" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A141" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B141" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A142" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B142" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A143" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B143" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A144" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B144" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B145" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A146" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B146" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A147" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B147" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A148" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B148" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A149" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B149" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A150" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B150" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A151" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B151" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A152" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B152" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A153" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B153" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A154" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B154" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A155" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B155" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A156" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B156" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A157" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B157" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A158" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B158" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A159" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B159" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A160" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B160" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A161" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B161" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A162" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B162" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A163" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B163" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A164" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B164" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A165" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B165" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A166" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B166" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A167" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B167" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A168" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B168" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A169" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B169" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A170" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B170" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A171" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B171" s="11">
+        <v>3.3962060000000003</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A172" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B172" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A173" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B173" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A174" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B174" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A175" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B175" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A176" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B176" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A177" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B177" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A178" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B178" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A179" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B179" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A180" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B180" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A181" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B181" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A182" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B182" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A183" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A184" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B184" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A185" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B185" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A186" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B186" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A187" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B187" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A188" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B188" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A189" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B189" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A190" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B190" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A191" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B191" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A192" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B192" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A193" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B193" s="11">
+        <v>3.3962060000000003</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A194" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B194" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A195" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B195" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A196" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B196" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A197" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B197" s="11">
+        <v>1.005455</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A198" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B198" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A199" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B199" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A200" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B200" s="13">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A201" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B201" s="11">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A202" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B202" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A203" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B203" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A204" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B204" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A205" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B205" s="11">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A206" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B206" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A207" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B207" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A208" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B208" s="13">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A209" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B209" s="11">
+        <v>0.49155599999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A210" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B210" s="13">
+        <v>0.98311199999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A211" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B211" s="11">
+        <v>3.3962050000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A212" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B212" s="13">
+        <v>1.6981030000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
@@ -1559,7 +3903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC33DFE9-8C65-4A33-8FAE-96323628CE2A}">
   <dimension ref="A1:D626"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-08 13:22
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A4F32F-7A52-4E0D-B3E3-1C2820711D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29FD8AC-D231-48E7-B703-107634929D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="grids_capacity" sheetId="4" r:id="rId1"/>
-    <sheet name="Veda" sheetId="1" r:id="rId2"/>
-    <sheet name="historical_data_long" sheetId="3" r:id="rId3"/>
+    <sheet name="Veda" sheetId="1" r:id="rId1"/>
+    <sheet name="historical_data_long" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="77">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -328,639 +327,6 @@
   </si>
   <si>
     <t>UC_RHSRT~2050</t>
-  </si>
-  <si>
-    <t>pasti</t>
-  </si>
-  <si>
-    <t>g_CH1-220-CH2-220</t>
-  </si>
-  <si>
-    <t>g_CH11-220-w147557680-220</t>
-  </si>
-  <si>
-    <t>g_CH12-220-w207993342-220</t>
-  </si>
-  <si>
-    <t>g_CH12-380-w207993342-380</t>
-  </si>
-  <si>
-    <t>g_CH13-220-CH12-220</t>
-  </si>
-  <si>
-    <t>g_CH13-220-w52738225-220</t>
-  </si>
-  <si>
-    <t>g_CH14-220-w212722603-220</t>
-  </si>
-  <si>
-    <t>g_CH14-220-w402053379-220</t>
-  </si>
-  <si>
-    <t>g_CH14-380-w50319857-380</t>
-  </si>
-  <si>
-    <t>g_CH15-220-w159527493-220</t>
-  </si>
-  <si>
-    <t>g_CH15-220-w97941869-220</t>
-  </si>
-  <si>
-    <t>g_CH17-380-w71500123-380</t>
-  </si>
-  <si>
-    <t>g_CH18-380-CH16-380</t>
-  </si>
-  <si>
-    <t>g_CH19-220-CH14-220</t>
-  </si>
-  <si>
-    <t>g_CH19-220-CH20-220</t>
-  </si>
-  <si>
-    <t>g_CH2-220-w50319857-220</t>
-  </si>
-  <si>
-    <t>g_CH20-220-CH19-220</t>
-  </si>
-  <si>
-    <t>g_CH21-220-w36348118-220</t>
-  </si>
-  <si>
-    <t>g_CH22-380-CH29-380</t>
-  </si>
-  <si>
-    <t>g_CH23-220-CH24-220</t>
-  </si>
-  <si>
-    <t>g_CH24-220-CH26-220</t>
-  </si>
-  <si>
-    <t>g_CH25-220-w240959264-220</t>
-  </si>
-  <si>
-    <t>g_CH26-220-CH28-220</t>
-  </si>
-  <si>
-    <t>g_CH27-220-CH25-220</t>
-  </si>
-  <si>
-    <t>g_CH27-220-w1086214433-220</t>
-  </si>
-  <si>
-    <t>g_CH28-220-w431234146-220</t>
-  </si>
-  <si>
-    <t>g_CH3-220-w281809991-220</t>
-  </si>
-  <si>
-    <t>g_CH30-380-CH33-380</t>
-  </si>
-  <si>
-    <t>g_CH30-380-w208780268-380</t>
-  </si>
-  <si>
-    <t>g_CH31-220-w132373704-220</t>
-  </si>
-  <si>
-    <t>g_CH32-220-w281803398-220</t>
-  </si>
-  <si>
-    <t>g_CH33-380-CH37-380</t>
-  </si>
-  <si>
-    <t>g_CH34-220-CH35-220</t>
-  </si>
-  <si>
-    <t>g_CH36-220-CH27-220</t>
-  </si>
-  <si>
-    <t>g_CH36-220-CH39-220</t>
-  </si>
-  <si>
-    <t>g_CH37-380-w207991759-380</t>
-  </si>
-  <si>
-    <t>g_CH38-220-CH39-220</t>
-  </si>
-  <si>
-    <t>g_CH38-220-w1092884227-220</t>
-  </si>
-  <si>
-    <t>g_CH39-220-CH36-220</t>
-  </si>
-  <si>
-    <t>g_CH4-220-CH9-220</t>
-  </si>
-  <si>
-    <t>g_CH4-220-w92873516-220</t>
-  </si>
-  <si>
-    <t>g_CH40-220-CH35-220</t>
-  </si>
-  <si>
-    <t>g_CH41-380-w207993342-380</t>
-  </si>
-  <si>
-    <t>g_CH41-380-w281804158-380</t>
-  </si>
-  <si>
-    <t>g_CH42-220-w969811258-220</t>
-  </si>
-  <si>
-    <t>g_CH43-220-CH44-220</t>
-  </si>
-  <si>
-    <t>g_CH43-220-w402055336-220</t>
-  </si>
-  <si>
-    <t>g_CH44-220-w234983117-220</t>
-  </si>
-  <si>
-    <t>g_CH45-220-CH29-220</t>
-  </si>
-  <si>
-    <t>g_CH46-220-CH47-220</t>
-  </si>
-  <si>
-    <t>g_CH47-220-w212722603-220</t>
-  </si>
-  <si>
-    <t>g_CH49-225-CH48-225</t>
-  </si>
-  <si>
-    <t>g_CH5-220-w89977424-220</t>
-  </si>
-  <si>
-    <t>g_CH50-220-w281804158-220</t>
-  </si>
-  <si>
-    <t>g_CH53-225-CH49-225</t>
-  </si>
-  <si>
-    <t>g_CH53-225-w55698557-225</t>
-  </si>
-  <si>
-    <t>g_CH56-220-CH58-220</t>
-  </si>
-  <si>
-    <t>g_CH56-220-w281815404-220</t>
-  </si>
-  <si>
-    <t>g_CH59-220-w281800404-220</t>
-  </si>
-  <si>
-    <t>g_CH6-220-CH3-220</t>
-  </si>
-  <si>
-    <t>g_CH60-225-CH53-225</t>
-  </si>
-  <si>
-    <t>g_CH7-220-w89405664-220</t>
-  </si>
-  <si>
-    <t>g_CH9-220-w455120191-220</t>
-  </si>
-  <si>
-    <t>g_r5378910-220-w1105061707-220</t>
-  </si>
-  <si>
-    <t>g_r7933294-380-CH30-380</t>
-  </si>
-  <si>
-    <t>g_r9310861-220-w11282314-220</t>
-  </si>
-  <si>
-    <t>g_w100662075-220-w210568055-220</t>
-  </si>
-  <si>
-    <t>g_w108257952-220-w33271433-220</t>
-  </si>
-  <si>
-    <t>g_w108257952-220-w35002638-220</t>
-  </si>
-  <si>
-    <t>g_w109037817-220-CH2-220</t>
-  </si>
-  <si>
-    <t>g_w109037817-380-w397960460-380</t>
-  </si>
-  <si>
-    <t>g_w1105061707-220-CH14-220</t>
-  </si>
-  <si>
-    <t>g_w1105061707-220-w402053379-220</t>
-  </si>
-  <si>
-    <t>g_w1105061707-220-w402055336-220</t>
-  </si>
-  <si>
-    <t>g_w111162936-220-CH31-220</t>
-  </si>
-  <si>
-    <t>g_w111162936-220-w55698557-220</t>
-  </si>
-  <si>
-    <t>g_w111162936-380-w936521586-380</t>
-  </si>
-  <si>
-    <t>g_w11282314-220-CH12-220</t>
-  </si>
-  <si>
-    <t>g_w11282314-220-CH6-220</t>
-  </si>
-  <si>
-    <t>g_w1208713169-220-w207993342-220</t>
-  </si>
-  <si>
-    <t>g_w1208713169-220-w212498548-220</t>
-  </si>
-  <si>
-    <t>g_w122720993-220-w1105061707-220</t>
-  </si>
-  <si>
-    <t>g_w127004407-380-CH14-380</t>
-  </si>
-  <si>
-    <t>g_w127004407-380-w1105061707-380</t>
-  </si>
-  <si>
-    <t>g_w127004407-380-w50319857-380</t>
-  </si>
-  <si>
-    <t>g_w1284913429-220-w165513396-220</t>
-  </si>
-  <si>
-    <t>g_w1327084723-220-CH42-220</t>
-  </si>
-  <si>
-    <t>g_w1327084723-220-w281800404-220</t>
-  </si>
-  <si>
-    <t>g_w140873735-220-CH23-220</t>
-  </si>
-  <si>
-    <t>g_w140873735-220-w130198336-220</t>
-  </si>
-  <si>
-    <t>g_w140873735-220-w35002638-220</t>
-  </si>
-  <si>
-    <t>g_w146225999-220-w35002638-220</t>
-  </si>
-  <si>
-    <t>g_w147557680-220-CH14-220</t>
-  </si>
-  <si>
-    <t>g_w147714395-220-CH3-220</t>
-  </si>
-  <si>
-    <t>g_w147714395-220-w22899676-220</t>
-  </si>
-  <si>
-    <t>g_w147714395-380-CH17-380</t>
-  </si>
-  <si>
-    <t>g_w147714395-380-w192677427-380</t>
-  </si>
-  <si>
-    <t>g_w148015471-220-r9310861-220</t>
-  </si>
-  <si>
-    <t>g_w148015471-220-w31308888-220</t>
-  </si>
-  <si>
-    <t>g_w159527493-220-w240959264-220</t>
-  </si>
-  <si>
-    <t>g_w161853746-220-r5378910-220</t>
-  </si>
-  <si>
-    <t>g_w161853746-220-w1105061707-220</t>
-  </si>
-  <si>
-    <t>g_w165254212-220-w147557680-220</t>
-  </si>
-  <si>
-    <t>g_w165513396-220-w33271433-220</t>
-  </si>
-  <si>
-    <t>g_w177392130-220-CH51-220</t>
-  </si>
-  <si>
-    <t>g_w177392130-220-CH52-220</t>
-  </si>
-  <si>
-    <t>g_w177392130-220-CH57-220</t>
-  </si>
-  <si>
-    <t>g_w177392130-400-CH51-400</t>
-  </si>
-  <si>
-    <t>g_w190819048-220-CH7-220</t>
-  </si>
-  <si>
-    <t>g_w190819048-220-w50319857-220</t>
-  </si>
-  <si>
-    <t>g_w192677427-220-CH13-220</t>
-  </si>
-  <si>
-    <t>g_w192677427-220-CH18-220</t>
-  </si>
-  <si>
-    <t>g_w192677427-220-w147714395-220</t>
-  </si>
-  <si>
-    <t>g_w192677427-220-w240575085-220</t>
-  </si>
-  <si>
-    <t>g_w192677427-380-CH16-380</t>
-  </si>
-  <si>
-    <t>g_w194258388-220-w122720993-220</t>
-  </si>
-  <si>
-    <t>g_w207993342-220-CH22-220</t>
-  </si>
-  <si>
-    <t>g_w208780268-380-w207993342-380</t>
-  </si>
-  <si>
-    <t>g_w209324991-220-w758315582-220</t>
-  </si>
-  <si>
-    <t>g_w210568055-220-w192677427-220</t>
-  </si>
-  <si>
-    <t>g_w210568055-220-w365556107-220</t>
-  </si>
-  <si>
-    <t>g_w210568055-380-CH16-380</t>
-  </si>
-  <si>
-    <t>g_w210568055-380-w71500123-380</t>
-  </si>
-  <si>
-    <t>g_w211907009-220-CH21-220</t>
-  </si>
-  <si>
-    <t>g_w211907009-220-w455120191-220</t>
-  </si>
-  <si>
-    <t>g_w212722603-220-w234983117-220</t>
-  </si>
-  <si>
-    <t>g_w212722603-220-w236819191-220</t>
-  </si>
-  <si>
-    <t>g_w212722603-380-w234983117-380</t>
-  </si>
-  <si>
-    <t>g_w22899676-220-CH3-220</t>
-  </si>
-  <si>
-    <t>g_w232662311-220-w111162936-220</t>
-  </si>
-  <si>
-    <t>g_w236819191-220-CH47-220</t>
-  </si>
-  <si>
-    <t>g_w236819191-220-w228003081-220</t>
-  </si>
-  <si>
-    <t>g_w238138373-380-w260211728-380</t>
-  </si>
-  <si>
-    <t>g_w239937062-220-CH52-220</t>
-  </si>
-  <si>
-    <t>g_w239937062-220-w132373704-220</t>
-  </si>
-  <si>
-    <t>g_w240575085-220-CH6-220</t>
-  </si>
-  <si>
-    <t>g_w240959264-220-CH20-220</t>
-  </si>
-  <si>
-    <t>g_w240959264-220-CH27-220</t>
-  </si>
-  <si>
-    <t>g_w240959264-220-w209324991-220</t>
-  </si>
-  <si>
-    <t>g_w242269161-220-CH14-220</t>
-  </si>
-  <si>
-    <t>g_w260211728-380-w936521586-380</t>
-  </si>
-  <si>
-    <t>g_w26166640-220-w758315582-220</t>
-  </si>
-  <si>
-    <t>g_w26843160-220-w92798668-220</t>
-  </si>
-  <si>
-    <t>g_w27107779-220-w147714395-220</t>
-  </si>
-  <si>
-    <t>g_w27435934-220-w109037817-220</t>
-  </si>
-  <si>
-    <t>g_w27435934-220-w30350721-220</t>
-  </si>
-  <si>
-    <t>g_w281799252-220-w52738225-220</t>
-  </si>
-  <si>
-    <t>g_w281800404-220-CH59-220</t>
-  </si>
-  <si>
-    <t>g_w281800404-220-w281815404-220</t>
-  </si>
-  <si>
-    <t>g_w281803398-220-CH50-220</t>
-  </si>
-  <si>
-    <t>g_w281809991-220-w26843160-220</t>
-  </si>
-  <si>
-    <t>g_w281815404-220-CH50-220</t>
-  </si>
-  <si>
-    <t>g_w281815404-220-CH58-220</t>
-  </si>
-  <si>
-    <t>g_w281815404-220-w35487135-220</t>
-  </si>
-  <si>
-    <t>g_w281822905-220-CH38-220</t>
-  </si>
-  <si>
-    <t>g_w281822905-220-CH42-220</t>
-  </si>
-  <si>
-    <t>g_w30350721-220-w356292116-220</t>
-  </si>
-  <si>
-    <t>g_w31308888-220-w89977424-220</t>
-  </si>
-  <si>
-    <t>g_w33271433-220-CH5-220</t>
-  </si>
-  <si>
-    <t>g_w35002638-220-CH15-220</t>
-  </si>
-  <si>
-    <t>g_w35002638-220-w140873735-220</t>
-  </si>
-  <si>
-    <t>g_w35002638-220-w242269161-220</t>
-  </si>
-  <si>
-    <t>g_w35002638-220-w281799252-220</t>
-  </si>
-  <si>
-    <t>g_w35002638-380-w52738225-380</t>
-  </si>
-  <si>
-    <t>g_w356292116-220-CH11-220</t>
-  </si>
-  <si>
-    <t>g_w356292116-220-w146225999-220</t>
-  </si>
-  <si>
-    <t>g_w356292116-220-w35002638-220</t>
-  </si>
-  <si>
-    <t>g_w356292116-220-w50319857-220</t>
-  </si>
-  <si>
-    <t>g_w356292116-380-w35002638-380</t>
-  </si>
-  <si>
-    <t>g_w356292116-380-w50319857-380</t>
-  </si>
-  <si>
-    <t>g_w35840165-380-w98648381-380</t>
-  </si>
-  <si>
-    <t>g_w364949845-220-w969819301-220</t>
-  </si>
-  <si>
-    <t>g_w364949845-380-CH34-380</t>
-  </si>
-  <si>
-    <t>g_w365556107-220-w71500123-220</t>
-  </si>
-  <si>
-    <t>g_w391577741-220-w391576135-220</t>
-  </si>
-  <si>
-    <t>g_w397960460-380-w50319857-380</t>
-  </si>
-  <si>
-    <t>g_w402053379-220-w190819048-220</t>
-  </si>
-  <si>
-    <t>g_w431234146-220-CH35-220</t>
-  </si>
-  <si>
-    <t>g_w431234146-220-w969811258-220</t>
-  </si>
-  <si>
-    <t>g_w44496892-220-CH31-220</t>
-  </si>
-  <si>
-    <t>g_w50319857-220-w98648381-220</t>
-  </si>
-  <si>
-    <t>g_w50319857-380-w35840165-380</t>
-  </si>
-  <si>
-    <t>g_w50319857-380-w98648381-380</t>
-  </si>
-  <si>
-    <t>g_w50561341-220-w147714395-220</t>
-  </si>
-  <si>
-    <t>g_w50561341-220-w87281514-220</t>
-  </si>
-  <si>
-    <t>g_w52738225-220-CH13-220</t>
-  </si>
-  <si>
-    <t>g_w52738225-380-CH12-380</t>
-  </si>
-  <si>
-    <t>g_w55695765-220-w111162936-220</t>
-  </si>
-  <si>
-    <t>g_w55698557-220-w194258388-220</t>
-  </si>
-  <si>
-    <t>g_w71500123-220-CH21-220</t>
-  </si>
-  <si>
-    <t>g_w71500123-380-w207993342-380</t>
-  </si>
-  <si>
-    <t>g_w758943072-220-w234983117-220</t>
-  </si>
-  <si>
-    <t>g_w802058337-220-w234983117-220</t>
-  </si>
-  <si>
-    <t>g_w802058337-220-w758943072-220</t>
-  </si>
-  <si>
-    <t>g_w802058337-225-CH60-225</t>
-  </si>
-  <si>
-    <t>g_w83861269-220-CH9-220</t>
-  </si>
-  <si>
-    <t>g_w89405664-220-w165513396-220</t>
-  </si>
-  <si>
-    <t>g_w89977424-220-CH5-220</t>
-  </si>
-  <si>
-    <t>g_w92798668-220-CH4-220</t>
-  </si>
-  <si>
-    <t>g_w92798668-220-w192677427-220</t>
-  </si>
-  <si>
-    <t>g_w92798668-220-w455120191-220</t>
-  </si>
-  <si>
-    <t>g_w936521586-380-w234983117-380</t>
-  </si>
-  <si>
-    <t>g_w969811258-380-w35002638-380</t>
-  </si>
-  <si>
-    <t>g_w969819301-220-CH46-220</t>
-  </si>
-  <si>
-    <t>g_w969819301-220-w391577741-220</t>
-  </si>
-  <si>
-    <t>g_w969819301-380-w364949845-380</t>
-  </si>
-  <si>
-    <t>g_w98648381-220-w165513396-220</t>
-  </si>
-  <si>
-    <t>g_w98648381-220-w27107779-220</t>
-  </si>
-  <si>
-    <t>g_w98648381-380-w147714395-380</t>
-  </si>
-  <si>
-    <t>g_w98648381-380-w165513396-380</t>
   </si>
 </sst>
 </file>
@@ -1445,1720 +811,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6B6990-516F-4858-B77B-B34C89415905}">
-  <dimension ref="A1:B212"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="28.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="13">
-        <v>1.4746679999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="11">
-        <v>1.4746679999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="13">
-        <v>1.0054560000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B56" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B57" s="11">
-        <v>1.005455</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B58" s="13">
-        <v>1.005455</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B60" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="B61" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B62" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B63" s="11">
-        <v>1.005455</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A64" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B64" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A65" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B65" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A66" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="B66" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A67" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B67" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A68" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A69" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B69" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A70" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B70" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A71" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B71" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A72" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B72" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A73" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B73" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A74" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B74" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B75" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A76" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B76" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A77" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B77" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A78" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B78" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A79" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A80" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B80" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A81" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B81" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A82" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B82" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A83" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B83" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A84" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B84" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A85" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B85" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A86" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B86" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A87" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="B87" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A88" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B88" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A89" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B89" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A90" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B90" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A91" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B91" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A92" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B92" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A93" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B93" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A94" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B94" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A95" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="B95" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A96" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B96" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A97" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B97" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A98" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B98" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A99" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="B99" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A100" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B100" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A101" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B101" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A102" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B102" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A103" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B103" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A104" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B104" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A105" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="B105" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A106" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B106" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A107" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="B107" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A108" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="B108" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A109" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B109" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A110" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B110" s="13">
-        <v>1.7874760000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A111" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B111" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A112" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B112" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A113" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B113" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A114" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B114" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A115" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B115" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A116" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B116" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A117" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B117" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A118" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B118" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A119" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B119" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A120" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="B120" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A121" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B121" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A122" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="B122" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A123" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B123" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A124" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="B124" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A125" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B125" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A126" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B126" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A127" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B127" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A128" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B128" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A129" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B129" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A130" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B130" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A131" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B131" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A132" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B132" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A133" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B133" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A134" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="B134" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A135" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B135" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A136" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B136" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A137" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B137" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A138" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="B138" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A139" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B139" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A140" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B140" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A141" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B141" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A142" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="B142" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A143" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B143" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A144" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B144" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A145" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B145" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A146" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="B146" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A147" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B147" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A148" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B148" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A149" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B149" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A150" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B150" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A151" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="B151" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A152" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="B152" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A153" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B153" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A154" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="B154" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A155" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="B155" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A156" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="B156" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A157" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="B157" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A158" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="B158" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A159" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B159" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A160" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="B160" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A161" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="B161" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A162" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="B162" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A163" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="B163" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A164" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="B164" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A165" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="B165" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A166" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="B166" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A167" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="B167" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A168" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="B168" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A169" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="B169" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A170" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="B170" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A171" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="B171" s="11">
-        <v>3.3962060000000003</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A172" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="B172" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A173" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="B173" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A174" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B174" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A175" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="B175" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A176" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="B176" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A177" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="B177" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A178" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B178" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A179" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="B179" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A180" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B180" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A181" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="B181" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A182" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="B182" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A183" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="B183" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A184" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="B184" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A185" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="B185" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A186" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="B186" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A187" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="B187" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A188" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="B188" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A189" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="B189" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A190" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="B190" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A191" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="B191" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A192" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="B192" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A193" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="B193" s="11">
-        <v>3.3962060000000003</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A194" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="B194" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A195" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="B195" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A196" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="B196" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A197" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="B197" s="11">
-        <v>1.005455</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A198" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B198" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A199" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="B199" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A200" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="B200" s="13">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A201" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="B201" s="11">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A202" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B202" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A203" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="B203" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A204" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B204" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A205" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="B205" s="11">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A206" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B206" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A207" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="B207" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A208" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="B208" s="13">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A209" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="B209" s="11">
-        <v>0.49155599999999999</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A210" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="B210" s="13">
-        <v>0.98311199999999999</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A211" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="B211" s="11">
-        <v>3.3962050000000001</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A212" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B212" s="13">
-        <v>1.6981030000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
@@ -3903,7 +1559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC33DFE9-8C65-4A33-8FAE-96323628CE2A}">
   <dimension ref="A1:D626"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-08 16:50
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC0D1D0-558A-454F-880F-5D5DE45CB59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6766674-BBF0-4924-980F-0233D0AB8B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="281">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -937,6 +937,9 @@
   </si>
   <si>
     <t>g_w969819301-220-w758943072-220</t>
+  </si>
+  <si>
+    <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by intuition · Accelerated with AI</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1000,8 +1003,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1023,6 +1033,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7F9FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF19375F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,7 +1086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1087,6 +1103,9 @@
     <xf numFmtId="2" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,1647 +1440,1664 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A67C6BA-690C-4B19-A860-39DCB4BD9EF0}">
-  <dimension ref="A1:B204"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB88B27-9ED3-4EE0-9618-6035A25562B6}">
+  <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="28.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="11">
+      <c r="C4" s="11">
         <v>2.1896590000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="13">
+      <c r="C5" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="11">
+      <c r="C6" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="13">
+      <c r="C7" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B8" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="11">
+      <c r="C8" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B9" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="13">
+      <c r="C9" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="11">
+      <c r="C10" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="13">
+      <c r="C11" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="11">
+      <c r="C12" s="11">
         <v>1.005455</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B13" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="13">
+      <c r="C13" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B14" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="11">
+      <c r="C14" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B15" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="13">
+      <c r="C15" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="11">
+      <c r="C16" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="13">
+      <c r="C17" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="11">
+      <c r="C18" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="13">
+      <c r="C19" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="11">
+      <c r="C20" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="12" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="13">
+      <c r="C21" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="11">
+      <c r="C22" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="13">
+      <c r="C23" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="11">
+      <c r="C24" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="13">
+      <c r="C25" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="11">
+      <c r="C26" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="13">
+      <c r="C27" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="11">
+      <c r="C28" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="12" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="13">
+      <c r="C29" s="13">
         <v>2.2790319999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="11">
+      <c r="C30" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="12" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="13">
+      <c r="C31" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="10" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="11">
+      <c r="C32" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="13">
+      <c r="C33" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="11">
+      <c r="C34" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="13">
+      <c r="C35" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" s="10" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="11">
+      <c r="C36" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="12" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="13">
+      <c r="C37" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="10" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="11">
+      <c r="C38" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="13">
+      <c r="C39" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" s="10" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="11">
+      <c r="C40" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="12" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="13">
+      <c r="C41" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="10" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="11">
+      <c r="C42" s="11">
         <v>3.8877609999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" s="12" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="13">
+      <c r="C43" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="10" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B43" s="11">
+      <c r="C44" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="13">
+      <c r="C45" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="10" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B45" s="11">
+      <c r="C46" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="12" t="s">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="13">
+      <c r="C47" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="10" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="11">
+      <c r="C48" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="12" t="s">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="13">
+      <c r="C49" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="11">
+      <c r="C50" s="11">
         <v>3.8877620000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B50" s="13">
+      <c r="C51" s="13">
         <v>2.1896590000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="10" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="11">
+      <c r="C52" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="12" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B52" s="13">
+      <c r="C53" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="10" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="11">
+      <c r="C54" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="12" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="13">
+      <c r="C55" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="10" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B55" s="11">
+      <c r="C56" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="12" t="s">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B56" s="13">
+      <c r="C57" s="13">
         <v>3.8877609999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="10" t="s">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="11">
+      <c r="C58" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="12" t="s">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="13">
+      <c r="C59" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" s="10" t="s">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B59" s="11">
+      <c r="C60" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="12" t="s">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B60" s="13">
+      <c r="C61" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="10" t="s">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B61" s="11">
+      <c r="C62" s="11">
         <v>3.3962060000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" s="12" t="s">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B62" s="13">
+      <c r="C63" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="10" t="s">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="11">
+      <c r="C64" s="11">
         <v>1.005455</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A64" s="12" t="s">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B64" s="13">
+      <c r="C65" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A65" s="10" t="s">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B65" s="11">
+      <c r="C66" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A66" s="12" t="s">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B66" s="13">
+      <c r="C67" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A67" s="10" t="s">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B67" s="11">
+      <c r="C68" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A68" s="12" t="s">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B69" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="13">
+      <c r="C69" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A69" s="10" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="11">
+      <c r="C70" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A70" s="12" t="s">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B70" s="13">
+      <c r="C71" s="13">
         <v>2.1896590000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A71" s="10" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="11">
+      <c r="C72" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A72" s="12" t="s">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B72" s="13">
+      <c r="C73" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A73" s="10" t="s">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="11">
+      <c r="C74" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A74" s="12" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B75" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B74" s="13">
+      <c r="C75" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" s="10" t="s">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B76" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B75" s="11">
+      <c r="C76" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A76" s="12" t="s">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B77" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B76" s="13">
+      <c r="C77" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A77" s="10" t="s">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B78" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="11">
+      <c r="C78" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A78" s="12" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B79" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="13">
+      <c r="C79" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A79" s="10" t="s">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B80" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B79" s="11">
+      <c r="C80" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A80" s="12" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B81" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B80" s="13">
+      <c r="C81" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A81" s="10" t="s">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B82" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B81" s="11">
+      <c r="C82" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A82" s="12" t="s">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B83" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="13">
+      <c r="C83" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A83" s="10" t="s">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B84" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B83" s="11">
+      <c r="C84" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A84" s="12" t="s">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B85" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="B84" s="13">
+      <c r="C85" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A85" s="10" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B86" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B85" s="11">
+      <c r="C86" s="11">
         <v>1.4746679999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A86" s="12" t="s">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B87" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B86" s="13">
+      <c r="C87" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A87" s="10" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B88" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B87" s="11">
+      <c r="C88" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A88" s="12" t="s">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B89" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B88" s="13">
+      <c r="C89" s="13">
         <v>1.4746679999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A89" s="10" t="s">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B90" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B89" s="11">
+      <c r="C90" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A90" s="12" t="s">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B91" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B90" s="13">
+      <c r="C91" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A91" s="10" t="s">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B92" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B91" s="11">
+      <c r="C92" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A92" s="12" t="s">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B93" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B92" s="13">
+      <c r="C93" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A93" s="10" t="s">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B94" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B93" s="11">
+      <c r="C94" s="11">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A94" s="12" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B95" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B94" s="13">
+      <c r="C95" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A95" s="10" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B96" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B95" s="11">
+      <c r="C96" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A96" s="12" t="s">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B97" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B96" s="13">
+      <c r="C97" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A97" s="10" t="s">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B98" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B97" s="11">
+      <c r="C98" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A98" s="12" t="s">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B99" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B98" s="13">
+      <c r="C99" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A99" s="10" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B100" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="B99" s="11">
+      <c r="C100" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A100" s="12" t="s">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B101" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B100" s="13">
+      <c r="C101" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A101" s="10" t="s">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B102" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="B101" s="11">
+      <c r="C102" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A102" s="12" t="s">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B103" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="B102" s="13">
+      <c r="C103" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A103" s="10" t="s">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B104" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B103" s="11">
+      <c r="C104" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A104" s="12" t="s">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B105" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="B104" s="13">
+      <c r="C105" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A105" s="10" t="s">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B106" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B105" s="11">
+      <c r="C106" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A106" s="12" t="s">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B107" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B106" s="13">
+      <c r="C107" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A107" s="10" t="s">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B108" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="B107" s="11">
+      <c r="C108" s="11">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A108" s="12" t="s">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B109" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B108" s="13">
+      <c r="C109" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A109" s="10" t="s">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B110" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B109" s="11">
+      <c r="C110" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A110" s="12" t="s">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B111" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B110" s="13">
+      <c r="C111" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A111" s="10" t="s">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B112" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B111" s="11">
+      <c r="C112" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A112" s="12" t="s">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B113" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B112" s="13">
+      <c r="C113" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A113" s="10" t="s">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B114" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B113" s="11">
+      <c r="C114" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A114" s="12" t="s">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B115" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B114" s="13">
+      <c r="C115" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A115" s="10" t="s">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B116" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B115" s="11">
+      <c r="C116" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A116" s="12" t="s">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B117" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B116" s="13">
+      <c r="C117" s="13">
         <v>1.0054560000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A117" s="10" t="s">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B118" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="B117" s="11">
+      <c r="C118" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A118" s="12" t="s">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B119" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="B118" s="13">
+      <c r="C119" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A119" s="10" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B120" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="B119" s="11">
+      <c r="C120" s="11">
         <v>1.005455</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A120" s="12" t="s">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B121" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B120" s="13">
+      <c r="C121" s="13">
         <v>1.005455</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A121" s="10" t="s">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B122" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B121" s="11">
+      <c r="C122" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A122" s="12" t="s">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B123" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B122" s="13">
+      <c r="C123" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A123" s="10" t="s">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B124" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B123" s="11">
+      <c r="C124" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A124" s="12" t="s">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B125" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B124" s="13">
+      <c r="C125" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A125" s="10" t="s">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B126" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B125" s="11">
+      <c r="C126" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A126" s="12" t="s">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B127" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B126" s="13">
+      <c r="C127" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A127" s="10" t="s">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B128" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="B127" s="11">
+      <c r="C128" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A128" s="12" t="s">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B129" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B128" s="13">
+      <c r="C129" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A129" s="10" t="s">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B130" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B129" s="11">
+      <c r="C130" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A130" s="12" t="s">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B131" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="B130" s="13">
+      <c r="C131" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A131" s="10" t="s">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B132" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B131" s="11">
+      <c r="C132" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A132" s="12" t="s">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B133" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B132" s="13">
+      <c r="C133" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A133" s="10" t="s">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B134" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B133" s="11">
+      <c r="C134" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A134" s="12" t="s">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B135" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B134" s="13">
+      <c r="C135" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A135" s="10" t="s">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B136" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B135" s="11">
+      <c r="C136" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A136" s="12" t="s">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B137" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B136" s="13">
+      <c r="C137" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A137" s="10" t="s">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B138" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B137" s="11">
+      <c r="C138" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A138" s="12" t="s">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B139" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B138" s="13">
+      <c r="C139" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A139" s="10" t="s">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B140" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="B139" s="11">
+      <c r="C140" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A140" s="12" t="s">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B141" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B140" s="13">
+      <c r="C141" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A141" s="10" t="s">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B142" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B141" s="11">
+      <c r="C142" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A142" s="12" t="s">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B143" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B142" s="13">
+      <c r="C143" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A143" s="10" t="s">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B144" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B143" s="11">
+      <c r="C144" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A144" s="12" t="s">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B145" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B144" s="13">
+      <c r="C145" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A145" s="10" t="s">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B146" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B145" s="11">
+      <c r="C146" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A146" s="12" t="s">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B147" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B146" s="13">
+      <c r="C147" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A147" s="10" t="s">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B148" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B147" s="11">
+      <c r="C148" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A148" s="12" t="s">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B149" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B148" s="13">
+      <c r="C149" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A149" s="10" t="s">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B150" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B149" s="11">
+      <c r="C150" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A150" s="12" t="s">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B151" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B150" s="13">
+      <c r="C151" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A151" s="10" t="s">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B152" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B151" s="11">
+      <c r="C152" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A152" s="12" t="s">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B153" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="B152" s="13">
+      <c r="C153" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A153" s="10" t="s">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B154" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="B153" s="11">
+      <c r="C154" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A154" s="12" t="s">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B155" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="B154" s="13">
+      <c r="C155" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A155" s="10" t="s">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B156" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B155" s="11">
+      <c r="C156" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A156" s="12" t="s">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B157" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="B156" s="13">
+      <c r="C157" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A157" s="10" t="s">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B158" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B157" s="11">
+      <c r="C158" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A158" s="12" t="s">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B159" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B158" s="13">
+      <c r="C159" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A159" s="10" t="s">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B160" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B159" s="11">
+      <c r="C160" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A160" s="12" t="s">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B161" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="B160" s="13">
+      <c r="C161" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A161" s="10" t="s">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B162" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B161" s="11">
+      <c r="C162" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A162" s="12" t="s">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B163" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B162" s="13">
+      <c r="C163" s="13">
         <v>3.3962050000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A163" s="10" t="s">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B164" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B163" s="11">
+      <c r="C164" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A164" s="12" t="s">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B165" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="B164" s="13">
+      <c r="C165" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A165" s="10" t="s">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B166" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B165" s="11">
+      <c r="C166" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A166" s="12" t="s">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B167" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="B166" s="13">
+      <c r="C167" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A167" s="10" t="s">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B168" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B167" s="11">
+      <c r="C168" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A168" s="12" t="s">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B169" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="B168" s="13">
+      <c r="C169" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A169" s="10" t="s">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B170" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B169" s="11">
+      <c r="C170" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A170" s="12" t="s">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B171" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="B170" s="13">
+      <c r="C171" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A171" s="10" t="s">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B172" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B171" s="11">
+      <c r="C172" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A172" s="12" t="s">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B173" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="B172" s="13">
+      <c r="C173" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A173" s="10" t="s">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B174" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B173" s="11">
+      <c r="C174" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A174" s="12" t="s">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B175" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B174" s="13">
+      <c r="C175" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A175" s="10" t="s">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B176" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B175" s="11">
+      <c r="C176" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A176" s="12" t="s">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B177" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B176" s="13">
+      <c r="C177" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A177" s="10" t="s">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B178" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B177" s="11">
+      <c r="C178" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A178" s="12" t="s">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B179" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="B178" s="13">
+      <c r="C179" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A179" s="10" t="s">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B180" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="B179" s="11">
+      <c r="C180" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A180" s="12" t="s">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B181" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B180" s="13">
+      <c r="C181" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A181" s="10" t="s">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B182" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="B181" s="11">
+      <c r="C182" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A182" s="12" t="s">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B183" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B182" s="13">
+      <c r="C183" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A183" s="10" t="s">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B184" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="B183" s="11">
+      <c r="C184" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A184" s="12" t="s">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B185" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B184" s="13">
+      <c r="C185" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A185" s="10" t="s">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B186" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="B185" s="11">
+      <c r="C186" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A186" s="12" t="s">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B187" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B186" s="13">
+      <c r="C187" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A187" s="10" t="s">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B188" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B187" s="11">
+      <c r="C188" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A188" s="12" t="s">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B189" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B188" s="13">
+      <c r="C189" s="13">
         <v>1.6981030000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A189" s="10" t="s">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B190" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="B189" s="11">
+      <c r="C190" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A190" s="12" t="s">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B191" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B190" s="13">
+      <c r="C191" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A191" s="10" t="s">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B192" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="B191" s="11">
+      <c r="C192" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A192" s="12" t="s">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B193" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B192" s="13">
+      <c r="C193" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A193" s="10" t="s">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B194" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="B193" s="11">
+      <c r="C194" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A194" s="12" t="s">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B195" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="B194" s="13">
+      <c r="C195" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A195" s="10" t="s">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B196" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="B195" s="11">
+      <c r="C196" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A196" s="12" t="s">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B197" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="B196" s="13">
+      <c r="C197" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A197" s="10" t="s">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B198" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="B197" s="11">
+      <c r="C198" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A198" s="12" t="s">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B199" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B198" s="13">
+      <c r="C199" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A199" s="10" t="s">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B200" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="B199" s="11">
+      <c r="C200" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A200" s="12" t="s">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B201" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B200" s="13">
+      <c r="C201" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A201" s="10" t="s">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B202" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="B201" s="11">
+      <c r="C202" s="11">
         <v>0.49155599999999999</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A202" s="12" t="s">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B203" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B202" s="13">
+      <c r="C203" s="13">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A203" s="10" t="s">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B204" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="B203" s="11">
+      <c r="C204" s="11">
         <v>0.98311199999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A204" s="12" t="s">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B205" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="B204" s="13">
+      <c r="C205" s="13">
         <v>0.49155599999999999</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-08 16:58
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6766674-BBF0-4924-980F-0233D0AB8B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA3F0A5D-0C13-45B0-A8A0-786C55435216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,7 +1440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB88B27-9ED3-4EE0-9618-6035A25562B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE316AC-9FE9-48E3-AB82-6CF78515C109}">
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-08 17:01
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA3F0A5D-0C13-45B0-A8A0-786C55435216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26A644A2-034C-4FA5-A956-566EC48F679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,7 +1440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE316AC-9FE9-48E3-AB82-6CF78515C109}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9AE5A2-1AE6-491D-B7B1-E444EB2AFD54}">
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-08 17:08
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26A644A2-034C-4FA5-A956-566EC48F679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A832D6D-7244-46BF-8D34-1568FCA1E2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,7 +1440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9AE5A2-1AE6-491D-B7B1-E444EB2AFD54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1457CEAD-B5AA-49DC-8644-BC51E7117BE3}">
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>